<commit_message>
Excel Output angepasst, Dateien aussortiert
</commit_message>
<xml_diff>
--- a/Ergebnisse.xlsx
+++ b/Ergebnisse.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
   <si>
     <t>Kernenergie</t>
   </si>
@@ -100,6 +100,30 @@
   </si>
   <si>
     <t>Pumpspeicher</t>
+  </si>
+  <si>
+    <t>FR_ex</t>
+  </si>
+  <si>
+    <t>NL_ex</t>
+  </si>
+  <si>
+    <t>PL_ex</t>
+  </si>
+  <si>
+    <t>SE_ex</t>
+  </si>
+  <si>
+    <t>NO_ex</t>
+  </si>
+  <si>
+    <t>Einspeicherung</t>
+  </si>
+  <si>
+    <t>Nachfrage</t>
+  </si>
+  <si>
+    <t>DE_ex</t>
   </si>
 </sst>
 </file>
@@ -451,13 +475,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:V25"/>
+  <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -524,8 +548,29 @@
       <c r="V1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:22">
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
       <c r="A2">
         <v>7695.0</v>
       </c>
@@ -592,8 +637,29 @@
       <c r="V2">
         <v>5514.660767000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:22">
+      <c r="W2">
+        <v>0.0</v>
+      </c>
+      <c r="X2">
+        <v>3200.0</v>
+      </c>
+      <c r="Y2">
+        <v>1000.0</v>
+      </c>
+      <c r="Z2">
+        <v>0.0</v>
+      </c>
+      <c r="AA2">
+        <v>0.0</v>
+      </c>
+      <c r="AB2">
+        <v>0.0</v>
+      </c>
+      <c r="AC2">
+        <v>42976.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29">
       <c r="A3">
         <v>7695.0</v>
       </c>
@@ -660,8 +726,29 @@
       <c r="V3">
         <v>835.6519660000013</v>
       </c>
-    </row>
-    <row r="4" spans="1:22">
+      <c r="W3">
+        <v>0.0</v>
+      </c>
+      <c r="X3">
+        <v>3200.0</v>
+      </c>
+      <c r="Y3">
+        <v>1000.0</v>
+      </c>
+      <c r="Z3">
+        <v>0.0</v>
+      </c>
+      <c r="AA3">
+        <v>0.0</v>
+      </c>
+      <c r="AB3">
+        <v>0.0</v>
+      </c>
+      <c r="AC3">
+        <v>41562.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29">
       <c r="A4">
         <v>7695.0</v>
       </c>
@@ -728,8 +815,29 @@
       <c r="V4">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="5" spans="1:22">
+      <c r="W4">
+        <v>0.0</v>
+      </c>
+      <c r="X4">
+        <v>3200.0</v>
+      </c>
+      <c r="Y4">
+        <v>1000.0</v>
+      </c>
+      <c r="Z4">
+        <v>0.0</v>
+      </c>
+      <c r="AA4">
+        <v>0.0</v>
+      </c>
+      <c r="AB4">
+        <v>0.0</v>
+      </c>
+      <c r="AC4">
+        <v>40100.0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29">
       <c r="A5">
         <v>7695.0</v>
       </c>
@@ -796,8 +904,29 @@
       <c r="V5">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="6" spans="1:22">
+      <c r="W5">
+        <v>0.0</v>
+      </c>
+      <c r="X5">
+        <v>3200.0</v>
+      </c>
+      <c r="Y5">
+        <v>1000.0</v>
+      </c>
+      <c r="Z5">
+        <v>0.0</v>
+      </c>
+      <c r="AA5">
+        <v>0.0</v>
+      </c>
+      <c r="AB5">
+        <v>748.2342136000043</v>
+      </c>
+      <c r="AC5">
+        <v>38883.0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29">
       <c r="A6">
         <v>6040.222914583338</v>
       </c>
@@ -864,8 +993,29 @@
       <c r="V6">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="7" spans="1:22">
+      <c r="W6">
+        <v>0.0</v>
+      </c>
+      <c r="X6">
+        <v>3200.0</v>
+      </c>
+      <c r="Y6">
+        <v>1000.0</v>
+      </c>
+      <c r="Z6">
+        <v>0.0</v>
+      </c>
+      <c r="AA6">
+        <v>0.0</v>
+      </c>
+      <c r="AB6">
+        <v>1227.5725452666702</v>
+      </c>
+      <c r="AC6">
+        <v>38806.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29">
       <c r="A7">
         <v>2818.9216989999986</v>
       </c>
@@ -932,8 +1082,29 @@
       <c r="V7">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="8" spans="1:22">
+      <c r="W7">
+        <v>0.0</v>
+      </c>
+      <c r="X7">
+        <v>3200.0</v>
+      </c>
+      <c r="Y7">
+        <v>1000.0</v>
+      </c>
+      <c r="Z7">
+        <v>0.0</v>
+      </c>
+      <c r="AA7">
+        <v>0.0</v>
+      </c>
+      <c r="AB7">
+        <v>0.0</v>
+      </c>
+      <c r="AC7">
+        <v>38593.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29">
       <c r="A8">
         <v>1004.7644660000005</v>
       </c>
@@ -1000,8 +1171,29 @@
       <c r="V8">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="9" spans="1:22">
+      <c r="W8">
+        <v>0.0</v>
+      </c>
+      <c r="X8">
+        <v>3200.0</v>
+      </c>
+      <c r="Y8">
+        <v>1000.0</v>
+      </c>
+      <c r="Z8">
+        <v>0.0</v>
+      </c>
+      <c r="AA8">
+        <v>0.0</v>
+      </c>
+      <c r="AB8">
+        <v>0.0</v>
+      </c>
+      <c r="AC8">
+        <v>38140.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29">
       <c r="A9">
         <v>7695.0</v>
       </c>
@@ -1068,8 +1260,29 @@
       <c r="V9">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="10" spans="1:22">
+      <c r="W9">
+        <v>0.0</v>
+      </c>
+      <c r="X9">
+        <v>3200.0</v>
+      </c>
+      <c r="Y9">
+        <v>1000.0</v>
+      </c>
+      <c r="Z9">
+        <v>0.0</v>
+      </c>
+      <c r="AA9">
+        <v>255.33333333333394</v>
+      </c>
+      <c r="AB9">
+        <v>5508.255974133335</v>
+      </c>
+      <c r="AC9">
+        <v>38742.0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29">
       <c r="A10">
         <v>716.7547437777812</v>
       </c>
@@ -1136,8 +1349,29 @@
       <c r="V10">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="11" spans="1:22">
+      <c r="W10">
+        <v>0.0</v>
+      </c>
+      <c r="X10">
+        <v>3200.0</v>
+      </c>
+      <c r="Y10">
+        <v>1000.0</v>
+      </c>
+      <c r="Z10">
+        <v>0.0</v>
+      </c>
+      <c r="AA10">
+        <v>545.9777777777763</v>
+      </c>
+      <c r="AB10">
+        <v>0.0</v>
+      </c>
+      <c r="AC10">
+        <v>39256.0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29">
       <c r="A11">
         <v>3526.6195059999973</v>
       </c>
@@ -1204,8 +1438,29 @@
       <c r="V11">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="12" spans="1:22">
+      <c r="W11">
+        <v>0.0</v>
+      </c>
+      <c r="X11">
+        <v>3200.0</v>
+      </c>
+      <c r="Y11">
+        <v>1000.0</v>
+      </c>
+      <c r="Z11">
+        <v>0.0</v>
+      </c>
+      <c r="AA11">
+        <v>841.1999999999987</v>
+      </c>
+      <c r="AB11">
+        <v>0.0</v>
+      </c>
+      <c r="AC11">
+        <v>42018.0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29">
       <c r="A12">
         <v>2932.690946444438</v>
       </c>
@@ -1272,8 +1527,29 @@
       <c r="V12">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="13" spans="1:22">
+      <c r="W12">
+        <v>0.0</v>
+      </c>
+      <c r="X12">
+        <v>3200.0</v>
+      </c>
+      <c r="Y12">
+        <v>1000.0</v>
+      </c>
+      <c r="Z12">
+        <v>0.0</v>
+      </c>
+      <c r="AA12">
+        <v>124.1444444444403</v>
+      </c>
+      <c r="AB12">
+        <v>0.0</v>
+      </c>
+      <c r="AC12">
+        <v>44533.0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29">
       <c r="A13">
         <v>3719.0306710000004</v>
       </c>
@@ -1340,8 +1616,29 @@
       <c r="V13">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="14" spans="1:22">
+      <c r="W13">
+        <v>0.0</v>
+      </c>
+      <c r="X13">
+        <v>3200.0</v>
+      </c>
+      <c r="Y13">
+        <v>1000.0</v>
+      </c>
+      <c r="Z13">
+        <v>0.0</v>
+      </c>
+      <c r="AA13">
+        <v>1400.0</v>
+      </c>
+      <c r="AB13">
+        <v>0.0</v>
+      </c>
+      <c r="AC13">
+        <v>47489.0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29">
       <c r="A14">
         <v>4129.839432111111</v>
       </c>
@@ -1408,8 +1705,29 @@
       <c r="V14">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="15" spans="1:22">
+      <c r="W14">
+        <v>0.0</v>
+      </c>
+      <c r="X14">
+        <v>3200.0</v>
+      </c>
+      <c r="Y14">
+        <v>1000.0</v>
+      </c>
+      <c r="Z14">
+        <v>0.0</v>
+      </c>
+      <c r="AA14">
+        <v>488.6111111111086</v>
+      </c>
+      <c r="AB14">
+        <v>0.0</v>
+      </c>
+      <c r="AC14">
+        <v>49261.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29">
       <c r="A15">
         <v>3372.423264888885</v>
       </c>
@@ -1476,8 +1794,29 @@
       <c r="V15">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="16" spans="1:22">
+      <c r="W15">
+        <v>0.0</v>
+      </c>
+      <c r="X15">
+        <v>3200.0</v>
+      </c>
+      <c r="Y15">
+        <v>1000.0</v>
+      </c>
+      <c r="Z15">
+        <v>0.0</v>
+      </c>
+      <c r="AA15">
+        <v>483.6888888888848</v>
+      </c>
+      <c r="AB15">
+        <v>0.0</v>
+      </c>
+      <c r="AC15">
+        <v>48832.0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29">
       <c r="A16">
         <v>4337.8061942222275</v>
       </c>
@@ -1544,8 +1883,29 @@
       <c r="V16">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="17" spans="1:22">
+      <c r="W16">
+        <v>0.0</v>
+      </c>
+      <c r="X16">
+        <v>3200.0</v>
+      </c>
+      <c r="Y16">
+        <v>1000.0</v>
+      </c>
+      <c r="Z16">
+        <v>0.0</v>
+      </c>
+      <c r="AA16">
+        <v>1204.4130232222242</v>
+      </c>
+      <c r="AB16">
+        <v>0.0</v>
+      </c>
+      <c r="AC16">
+        <v>48595.0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29">
       <c r="A17">
         <v>5923.830070000004</v>
       </c>
@@ -1612,8 +1972,29 @@
       <c r="V17">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="18" spans="1:22">
+      <c r="W17">
+        <v>0.0</v>
+      </c>
+      <c r="X17">
+        <v>3200.0</v>
+      </c>
+      <c r="Y17">
+        <v>1000.0</v>
+      </c>
+      <c r="Z17">
+        <v>0.0</v>
+      </c>
+      <c r="AA17">
+        <v>1400.0</v>
+      </c>
+      <c r="AB17">
+        <v>0.0</v>
+      </c>
+      <c r="AC17">
+        <v>48826.0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29">
       <c r="A18">
         <v>7042.612293000006</v>
       </c>
@@ -1680,8 +2061,29 @@
       <c r="V18">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="19" spans="1:22">
+      <c r="W18">
+        <v>0.0</v>
+      </c>
+      <c r="X18">
+        <v>3200.0</v>
+      </c>
+      <c r="Y18">
+        <v>1000.0</v>
+      </c>
+      <c r="Z18">
+        <v>0.0</v>
+      </c>
+      <c r="AA18">
+        <v>1400.0</v>
+      </c>
+      <c r="AB18">
+        <v>0.0</v>
+      </c>
+      <c r="AC18">
+        <v>50626.0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29">
       <c r="A19">
         <v>7695.0</v>
       </c>
@@ -1748,8 +2150,29 @@
       <c r="V19">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="20" spans="1:22">
+      <c r="W19">
+        <v>0.0</v>
+      </c>
+      <c r="X19">
+        <v>3200.0</v>
+      </c>
+      <c r="Y19">
+        <v>1000.0</v>
+      </c>
+      <c r="Z19">
+        <v>0.0</v>
+      </c>
+      <c r="AA19">
+        <v>1400.0</v>
+      </c>
+      <c r="AB19">
+        <v>0.0</v>
+      </c>
+      <c r="AC19">
+        <v>53793.0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29">
       <c r="A20">
         <v>7695.0</v>
       </c>
@@ -1816,8 +2239,29 @@
       <c r="V20">
         <v>669.0966990000015</v>
       </c>
-    </row>
-    <row r="21" spans="1:22">
+      <c r="W20">
+        <v>0.0</v>
+      </c>
+      <c r="X20">
+        <v>3200.0</v>
+      </c>
+      <c r="Y20">
+        <v>1000.0</v>
+      </c>
+      <c r="Z20">
+        <v>0.0</v>
+      </c>
+      <c r="AA20">
+        <v>0.0</v>
+      </c>
+      <c r="AB20">
+        <v>0.0</v>
+      </c>
+      <c r="AC20">
+        <v>54371.0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29">
       <c r="A21">
         <v>7695.0</v>
       </c>
@@ -1884,8 +2328,29 @@
       <c r="V21">
         <v>464.65330100000574</v>
       </c>
-    </row>
-    <row r="22" spans="1:22">
+      <c r="W21">
+        <v>0.0</v>
+      </c>
+      <c r="X21">
+        <v>3200.0</v>
+      </c>
+      <c r="Y21">
+        <v>1000.0</v>
+      </c>
+      <c r="Z21">
+        <v>0.0</v>
+      </c>
+      <c r="AA21">
+        <v>0.0</v>
+      </c>
+      <c r="AB21">
+        <v>0.0</v>
+      </c>
+      <c r="AC21">
+        <v>53815.0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29">
       <c r="A22">
         <v>7695.0</v>
       </c>
@@ -1952,8 +2417,29 @@
       <c r="V22">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="23" spans="1:22">
+      <c r="W22">
+        <v>0.0</v>
+      </c>
+      <c r="X22">
+        <v>3200.0</v>
+      </c>
+      <c r="Y22">
+        <v>1000.0</v>
+      </c>
+      <c r="Z22">
+        <v>0.0</v>
+      </c>
+      <c r="AA22">
+        <v>1312.6841989999957</v>
+      </c>
+      <c r="AB22">
+        <v>0.0</v>
+      </c>
+      <c r="AC22">
+        <v>51609.0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29">
       <c r="A23">
         <v>5360.700865666669</v>
       </c>
@@ -2020,8 +2506,29 @@
       <c r="V23">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="24" spans="1:22">
+      <c r="W23">
+        <v>0.0</v>
+      </c>
+      <c r="X23">
+        <v>3200.0</v>
+      </c>
+      <c r="Y23">
+        <v>1000.0</v>
+      </c>
+      <c r="Z23">
+        <v>0.0</v>
+      </c>
+      <c r="AA23">
+        <v>404.8666666666645</v>
+      </c>
+      <c r="AB23">
+        <v>0.0</v>
+      </c>
+      <c r="AC23">
+        <v>49698.0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29">
       <c r="A24">
         <v>6390.979166666661</v>
       </c>
@@ -2088,8 +2595,29 @@
       <c r="V24">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="25" spans="1:22">
+      <c r="W24">
+        <v>0.0</v>
+      </c>
+      <c r="X24">
+        <v>3200.0</v>
+      </c>
+      <c r="Y24">
+        <v>1000.0</v>
+      </c>
+      <c r="Z24">
+        <v>0.0</v>
+      </c>
+      <c r="AA24">
+        <v>1214.9666666666637</v>
+      </c>
+      <c r="AB24">
+        <v>0.0</v>
+      </c>
+      <c r="AC24">
+        <v>48859.0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29">
       <c r="A25">
         <v>4081.0577562222225</v>
       </c>
@@ -2155,6 +2683,27 @@
       </c>
       <c r="V25">
         <v>0.0</v>
+      </c>
+      <c r="W25">
+        <v>0.0</v>
+      </c>
+      <c r="X25">
+        <v>3200.0</v>
+      </c>
+      <c r="Y25">
+        <v>1000.0</v>
+      </c>
+      <c r="Z25">
+        <v>0.0</v>
+      </c>
+      <c r="AA25">
+        <v>1262.0222222222203</v>
+      </c>
+      <c r="AB25">
+        <v>0.0</v>
+      </c>
+      <c r="AC25">
+        <v>46093.0</v>
       </c>
     </row>
   </sheetData>
@@ -2677,13 +3226,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:V25"/>
+  <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2750,8 +3299,29 @@
       <c r="V1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:22">
+      <c r="W1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
       <c r="A2">
         <v>54055.0</v>
       </c>
@@ -2818,8 +3388,29 @@
       <c r="V2">
         <v>649.0</v>
       </c>
-    </row>
-    <row r="3" spans="1:22">
+      <c r="W2">
+        <v>0.0</v>
+      </c>
+      <c r="X2">
+        <v>800.0</v>
+      </c>
+      <c r="Y2">
+        <v>0.0</v>
+      </c>
+      <c r="Z2">
+        <v>0.0</v>
+      </c>
+      <c r="AA2">
+        <v>0.0</v>
+      </c>
+      <c r="AB2">
+        <v>0.0</v>
+      </c>
+      <c r="AC2">
+        <v>62176.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29">
       <c r="A3">
         <v>54055.0</v>
       </c>
@@ -2886,8 +3477,29 @@
       <c r="V3">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="4" spans="1:22">
+      <c r="W3">
+        <v>1241.0</v>
+      </c>
+      <c r="X3">
+        <v>800.0</v>
+      </c>
+      <c r="Y3">
+        <v>0.0</v>
+      </c>
+      <c r="Z3">
+        <v>0.0</v>
+      </c>
+      <c r="AA3">
+        <v>0.0</v>
+      </c>
+      <c r="AB3">
+        <v>0.0</v>
+      </c>
+      <c r="AC3">
+        <v>60301.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29">
       <c r="A4">
         <v>54055.0</v>
       </c>
@@ -2954,8 +3566,29 @@
       <c r="V4">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="5" spans="1:22">
+      <c r="W4">
+        <v>2015.7061488888867</v>
+      </c>
+      <c r="X4">
+        <v>800.0</v>
+      </c>
+      <c r="Y4">
+        <v>0.0</v>
+      </c>
+      <c r="Z4">
+        <v>0.0</v>
+      </c>
+      <c r="AA4">
+        <v>0.0</v>
+      </c>
+      <c r="AB4">
+        <v>733.0350808888891</v>
+      </c>
+      <c r="AC4">
+        <v>58540.0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29">
       <c r="A5">
         <v>48484.19226</v>
       </c>
@@ -3022,8 +3655,29 @@
       <c r="V5">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="6" spans="1:22">
+      <c r="W5">
+        <v>0.0</v>
+      </c>
+      <c r="X5">
+        <v>800.0</v>
+      </c>
+      <c r="Y5">
+        <v>0.0</v>
+      </c>
+      <c r="Z5">
+        <v>0.0</v>
+      </c>
+      <c r="AA5">
+        <v>0.0</v>
+      </c>
+      <c r="AB5">
+        <v>596.9538080000038</v>
+      </c>
+      <c r="AC5">
+        <v>55144.0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29">
       <c r="A6">
         <v>45533.0</v>
       </c>
@@ -3090,8 +3744,29 @@
       <c r="V6">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="7" spans="1:22">
+      <c r="W6">
+        <v>0.0</v>
+      </c>
+      <c r="X6">
+        <v>800.0</v>
+      </c>
+      <c r="Y6">
+        <v>0.0</v>
+      </c>
+      <c r="Z6">
+        <v>0.0</v>
+      </c>
+      <c r="AA6">
+        <v>0.0</v>
+      </c>
+      <c r="AB6">
+        <v>0.0</v>
+      </c>
+      <c r="AC6">
+        <v>52978.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29">
       <c r="A7">
         <v>45015.0</v>
       </c>
@@ -3158,8 +3833,29 @@
       <c r="V7">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="8" spans="1:22">
+      <c r="W7">
+        <v>0.0</v>
+      </c>
+      <c r="X7">
+        <v>800.0</v>
+      </c>
+      <c r="Y7">
+        <v>0.0</v>
+      </c>
+      <c r="Z7">
+        <v>0.0</v>
+      </c>
+      <c r="AA7">
+        <v>0.0</v>
+      </c>
+      <c r="AB7">
+        <v>0.0</v>
+      </c>
+      <c r="AC7">
+        <v>52584.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29">
       <c r="A8">
         <v>45237.0</v>
       </c>
@@ -3226,8 +3922,29 @@
       <c r="V8">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="9" spans="1:22">
+      <c r="W8">
+        <v>0.0</v>
+      </c>
+      <c r="X8">
+        <v>800.0</v>
+      </c>
+      <c r="Y8">
+        <v>0.0</v>
+      </c>
+      <c r="Z8">
+        <v>0.0</v>
+      </c>
+      <c r="AA8">
+        <v>0.0</v>
+      </c>
+      <c r="AB8">
+        <v>0.0</v>
+      </c>
+      <c r="AC8">
+        <v>52881.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29">
       <c r="A9">
         <v>45543.0</v>
       </c>
@@ -3294,8 +4011,29 @@
       <c r="V9">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="10" spans="1:22">
+      <c r="W9">
+        <v>0.0</v>
+      </c>
+      <c r="X9">
+        <v>800.0</v>
+      </c>
+      <c r="Y9">
+        <v>0.0</v>
+      </c>
+      <c r="Z9">
+        <v>0.0</v>
+      </c>
+      <c r="AA9">
+        <v>0.0</v>
+      </c>
+      <c r="AB9">
+        <v>0.0</v>
+      </c>
+      <c r="AC9">
+        <v>53173.0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29">
       <c r="A10">
         <v>45217.0</v>
       </c>
@@ -3362,8 +4100,29 @@
       <c r="V10">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="11" spans="1:22">
+      <c r="W10">
+        <v>0.0</v>
+      </c>
+      <c r="X10">
+        <v>800.0</v>
+      </c>
+      <c r="Y10">
+        <v>0.0</v>
+      </c>
+      <c r="Z10">
+        <v>0.0</v>
+      </c>
+      <c r="AA10">
+        <v>0.0</v>
+      </c>
+      <c r="AB10">
+        <v>0.0</v>
+      </c>
+      <c r="AC10">
+        <v>52929.0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29">
       <c r="A11">
         <v>45807.0</v>
       </c>
@@ -3430,8 +4189,29 @@
       <c r="V11">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="12" spans="1:22">
+      <c r="W11">
+        <v>0.0</v>
+      </c>
+      <c r="X11">
+        <v>800.0</v>
+      </c>
+      <c r="Y11">
+        <v>0.0</v>
+      </c>
+      <c r="Z11">
+        <v>0.0</v>
+      </c>
+      <c r="AA11">
+        <v>0.0</v>
+      </c>
+      <c r="AB11">
+        <v>0.0</v>
+      </c>
+      <c r="AC11">
+        <v>53830.0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29">
       <c r="A12">
         <v>47171.0</v>
       </c>
@@ -3498,8 +4278,29 @@
       <c r="V12">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="13" spans="1:22">
+      <c r="W12">
+        <v>0.0</v>
+      </c>
+      <c r="X12">
+        <v>800.0</v>
+      </c>
+      <c r="Y12">
+        <v>0.0</v>
+      </c>
+      <c r="Z12">
+        <v>0.0</v>
+      </c>
+      <c r="AA12">
+        <v>0.0</v>
+      </c>
+      <c r="AB12">
+        <v>0.0</v>
+      </c>
+      <c r="AC12">
+        <v>55677.0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29">
       <c r="A13">
         <v>48814.0</v>
       </c>
@@ -3566,8 +4367,29 @@
       <c r="V13">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="14" spans="1:22">
+      <c r="W13">
+        <v>0.0</v>
+      </c>
+      <c r="X13">
+        <v>800.0</v>
+      </c>
+      <c r="Y13">
+        <v>0.0</v>
+      </c>
+      <c r="Z13">
+        <v>0.0</v>
+      </c>
+      <c r="AA13">
+        <v>0.0</v>
+      </c>
+      <c r="AB13">
+        <v>0.0</v>
+      </c>
+      <c r="AC13">
+        <v>57722.0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29">
       <c r="A14">
         <v>51184.0</v>
       </c>
@@ -3634,8 +4456,29 @@
       <c r="V14">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="15" spans="1:22">
+      <c r="W14">
+        <v>0.0</v>
+      </c>
+      <c r="X14">
+        <v>800.0</v>
+      </c>
+      <c r="Y14">
+        <v>0.0</v>
+      </c>
+      <c r="Z14">
+        <v>0.0</v>
+      </c>
+      <c r="AA14">
+        <v>0.0</v>
+      </c>
+      <c r="AB14">
+        <v>0.0</v>
+      </c>
+      <c r="AC14">
+        <v>60387.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29">
       <c r="A15">
         <v>50461.0</v>
       </c>
@@ -3702,8 +4545,29 @@
       <c r="V15">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="16" spans="1:22">
+      <c r="W15">
+        <v>0.0</v>
+      </c>
+      <c r="X15">
+        <v>800.0</v>
+      </c>
+      <c r="Y15">
+        <v>0.0</v>
+      </c>
+      <c r="Z15">
+        <v>0.0</v>
+      </c>
+      <c r="AA15">
+        <v>0.0</v>
+      </c>
+      <c r="AB15">
+        <v>0.0</v>
+      </c>
+      <c r="AC15">
+        <v>60029.0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29">
       <c r="A16">
         <v>48557.0</v>
       </c>
@@ -3770,8 +4634,29 @@
       <c r="V16">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="17" spans="1:22">
+      <c r="W16">
+        <v>0.0</v>
+      </c>
+      <c r="X16">
+        <v>800.0</v>
+      </c>
+      <c r="Y16">
+        <v>0.0</v>
+      </c>
+      <c r="Z16">
+        <v>0.0</v>
+      </c>
+      <c r="AA16">
+        <v>0.0</v>
+      </c>
+      <c r="AB16">
+        <v>0.0</v>
+      </c>
+      <c r="AC16">
+        <v>57977.0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29">
       <c r="A17">
         <v>47857.0</v>
       </c>
@@ -3838,8 +4723,29 @@
       <c r="V17">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="18" spans="1:22">
+      <c r="W17">
+        <v>0.0</v>
+      </c>
+      <c r="X17">
+        <v>800.0</v>
+      </c>
+      <c r="Y17">
+        <v>0.0</v>
+      </c>
+      <c r="Z17">
+        <v>0.0</v>
+      </c>
+      <c r="AA17">
+        <v>0.0</v>
+      </c>
+      <c r="AB17">
+        <v>0.0</v>
+      </c>
+      <c r="AC17">
+        <v>56719.0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29">
       <c r="A18">
         <v>48364.0</v>
       </c>
@@ -3906,8 +4812,29 @@
       <c r="V18">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="19" spans="1:22">
+      <c r="W18">
+        <v>0.0</v>
+      </c>
+      <c r="X18">
+        <v>800.0</v>
+      </c>
+      <c r="Y18">
+        <v>0.0</v>
+      </c>
+      <c r="Z18">
+        <v>0.0</v>
+      </c>
+      <c r="AA18">
+        <v>0.0</v>
+      </c>
+      <c r="AB18">
+        <v>0.0</v>
+      </c>
+      <c r="AC18">
+        <v>56642.0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29">
       <c r="A19">
         <v>54055.0</v>
       </c>
@@ -3974,8 +4901,29 @@
       <c r="V19">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="20" spans="1:22">
+      <c r="W19">
+        <v>1632.9861111111095</v>
+      </c>
+      <c r="X19">
+        <v>800.0</v>
+      </c>
+      <c r="Y19">
+        <v>0.0</v>
+      </c>
+      <c r="Z19">
+        <v>0.0</v>
+      </c>
+      <c r="AA19">
+        <v>0.0</v>
+      </c>
+      <c r="AB19">
+        <v>900.0111111111064</v>
+      </c>
+      <c r="AC19">
+        <v>59439.0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29">
       <c r="A20">
         <v>54055.0</v>
       </c>
@@ -4042,8 +4990,29 @@
       <c r="V20">
         <v>341.0</v>
       </c>
-    </row>
-    <row r="21" spans="1:22">
+      <c r="W20">
+        <v>0.0</v>
+      </c>
+      <c r="X20">
+        <v>800.0</v>
+      </c>
+      <c r="Y20">
+        <v>0.0</v>
+      </c>
+      <c r="Z20">
+        <v>0.0</v>
+      </c>
+      <c r="AA20">
+        <v>0.0</v>
+      </c>
+      <c r="AB20">
+        <v>0.0</v>
+      </c>
+      <c r="AC20">
+        <v>62690.0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29">
       <c r="A21">
         <v>54055.0</v>
       </c>
@@ -4110,8 +5079,29 @@
       <c r="V21">
         <v>1240.0</v>
       </c>
-    </row>
-    <row r="22" spans="1:22">
+      <c r="W21">
+        <v>0.0</v>
+      </c>
+      <c r="X21">
+        <v>800.0</v>
+      </c>
+      <c r="Y21">
+        <v>0.0</v>
+      </c>
+      <c r="Z21">
+        <v>0.0</v>
+      </c>
+      <c r="AA21">
+        <v>0.0</v>
+      </c>
+      <c r="AB21">
+        <v>0.0</v>
+      </c>
+      <c r="AC21">
+        <v>63741.0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29">
       <c r="A22">
         <v>53738.0</v>
       </c>
@@ -4178,8 +5168,29 @@
       <c r="V22">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="23" spans="1:22">
+      <c r="W22">
+        <v>0.0</v>
+      </c>
+      <c r="X22">
+        <v>800.0</v>
+      </c>
+      <c r="Y22">
+        <v>0.0</v>
+      </c>
+      <c r="Z22">
+        <v>0.0</v>
+      </c>
+      <c r="AA22">
+        <v>0.0</v>
+      </c>
+      <c r="AB22">
+        <v>0.0</v>
+      </c>
+      <c r="AC22">
+        <v>62360.0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29">
       <c r="A23">
         <v>51292.0</v>
       </c>
@@ -4246,8 +5257,29 @@
       <c r="V23">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="24" spans="1:22">
+      <c r="W23">
+        <v>0.0</v>
+      </c>
+      <c r="X23">
+        <v>800.0</v>
+      </c>
+      <c r="Y23">
+        <v>0.0</v>
+      </c>
+      <c r="Z23">
+        <v>0.0</v>
+      </c>
+      <c r="AA23">
+        <v>0.0</v>
+      </c>
+      <c r="AB23">
+        <v>0.0</v>
+      </c>
+      <c r="AC23">
+        <v>60160.0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29">
       <c r="A24">
         <v>52119.0</v>
       </c>
@@ -4314,8 +5346,29 @@
       <c r="V24">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="25" spans="1:22">
+      <c r="W24">
+        <v>0.0</v>
+      </c>
+      <c r="X24">
+        <v>800.0</v>
+      </c>
+      <c r="Y24">
+        <v>0.0</v>
+      </c>
+      <c r="Z24">
+        <v>0.0</v>
+      </c>
+      <c r="AA24">
+        <v>0.0</v>
+      </c>
+      <c r="AB24">
+        <v>0.0</v>
+      </c>
+      <c r="AC24">
+        <v>60983.0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29">
       <c r="A25">
         <v>52902.0</v>
       </c>
@@ -4381,6 +5434,27 @@
       </c>
       <c r="V25">
         <v>0.0</v>
+      </c>
+      <c r="W25">
+        <v>0.0</v>
+      </c>
+      <c r="X25">
+        <v>800.0</v>
+      </c>
+      <c r="Y25">
+        <v>0.0</v>
+      </c>
+      <c r="Z25">
+        <v>0.0</v>
+      </c>
+      <c r="AA25">
+        <v>0.0</v>
+      </c>
+      <c r="AB25">
+        <v>0.0</v>
+      </c>
+      <c r="AC25">
+        <v>61763.0</v>
       </c>
     </row>
   </sheetData>
@@ -4390,13 +5464,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:V25"/>
+  <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4463,8 +5537,29 @@
       <c r="V1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:22">
+      <c r="W1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
       <c r="A2">
         <v>457.9</v>
       </c>
@@ -4531,8 +5626,29 @@
       <c r="V2">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="3" spans="1:22">
+      <c r="W2">
+        <v>0.0</v>
+      </c>
+      <c r="X2">
+        <v>0.0</v>
+      </c>
+      <c r="Y2">
+        <v>0.0</v>
+      </c>
+      <c r="Z2">
+        <v>0.0</v>
+      </c>
+      <c r="AA2">
+        <v>0.0</v>
+      </c>
+      <c r="AB2">
+        <v>0.0</v>
+      </c>
+      <c r="AC2">
+        <v>11285.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29">
       <c r="A3">
         <v>457.9</v>
       </c>
@@ -4599,8 +5715,29 @@
       <c r="V3">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="4" spans="1:22">
+      <c r="W3">
+        <v>0.0</v>
+      </c>
+      <c r="X3">
+        <v>0.0</v>
+      </c>
+      <c r="Y3">
+        <v>0.0</v>
+      </c>
+      <c r="Z3">
+        <v>0.0</v>
+      </c>
+      <c r="AA3">
+        <v>0.0</v>
+      </c>
+      <c r="AB3">
+        <v>0.0</v>
+      </c>
+      <c r="AC3">
+        <v>11194.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29">
       <c r="A4">
         <v>457.9</v>
       </c>
@@ -4667,8 +5804,29 @@
       <c r="V4">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="5" spans="1:22">
+      <c r="W4">
+        <v>0.0</v>
+      </c>
+      <c r="X4">
+        <v>0.0</v>
+      </c>
+      <c r="Y4">
+        <v>0.0</v>
+      </c>
+      <c r="Z4">
+        <v>0.0</v>
+      </c>
+      <c r="AA4">
+        <v>0.0</v>
+      </c>
+      <c r="AB4">
+        <v>0.0</v>
+      </c>
+      <c r="AC4">
+        <v>10933.0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29">
       <c r="A5">
         <v>457.9</v>
       </c>
@@ -4735,8 +5893,29 @@
       <c r="V5">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="6" spans="1:22">
+      <c r="W5">
+        <v>0.0</v>
+      </c>
+      <c r="X5">
+        <v>0.0</v>
+      </c>
+      <c r="Y5">
+        <v>0.0</v>
+      </c>
+      <c r="Z5">
+        <v>0.0</v>
+      </c>
+      <c r="AA5">
+        <v>0.0</v>
+      </c>
+      <c r="AB5">
+        <v>0.0</v>
+      </c>
+      <c r="AC5">
+        <v>10667.0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29">
       <c r="A6">
         <v>457.9</v>
       </c>
@@ -4803,8 +5982,29 @@
       <c r="V6">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="7" spans="1:22">
+      <c r="W6">
+        <v>0.0</v>
+      </c>
+      <c r="X6">
+        <v>0.0</v>
+      </c>
+      <c r="Y6">
+        <v>0.0</v>
+      </c>
+      <c r="Z6">
+        <v>0.0</v>
+      </c>
+      <c r="AA6">
+        <v>0.0</v>
+      </c>
+      <c r="AB6">
+        <v>0.0</v>
+      </c>
+      <c r="AC6">
+        <v>10413.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29">
       <c r="A7">
         <v>457.9</v>
       </c>
@@ -4871,8 +6071,29 @@
       <c r="V7">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="8" spans="1:22">
+      <c r="W7">
+        <v>0.0</v>
+      </c>
+      <c r="X7">
+        <v>0.0</v>
+      </c>
+      <c r="Y7">
+        <v>0.0</v>
+      </c>
+      <c r="Z7">
+        <v>0.0</v>
+      </c>
+      <c r="AA7">
+        <v>0.0</v>
+      </c>
+      <c r="AB7">
+        <v>0.0</v>
+      </c>
+      <c r="AC7">
+        <v>10441.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29">
       <c r="A8">
         <v>457.9</v>
       </c>
@@ -4939,8 +6160,29 @@
       <c r="V8">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="9" spans="1:22">
+      <c r="W8">
+        <v>0.0</v>
+      </c>
+      <c r="X8">
+        <v>0.0</v>
+      </c>
+      <c r="Y8">
+        <v>0.0</v>
+      </c>
+      <c r="Z8">
+        <v>0.0</v>
+      </c>
+      <c r="AA8">
+        <v>0.0</v>
+      </c>
+      <c r="AB8">
+        <v>0.0</v>
+      </c>
+      <c r="AC8">
+        <v>10670.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29">
       <c r="A9">
         <v>457.9</v>
       </c>
@@ -5007,8 +6249,29 @@
       <c r="V9">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="10" spans="1:22">
+      <c r="W9">
+        <v>0.0</v>
+      </c>
+      <c r="X9">
+        <v>0.0</v>
+      </c>
+      <c r="Y9">
+        <v>0.0</v>
+      </c>
+      <c r="Z9">
+        <v>0.0</v>
+      </c>
+      <c r="AA9">
+        <v>0.0</v>
+      </c>
+      <c r="AB9">
+        <v>0.0</v>
+      </c>
+      <c r="AC9">
+        <v>10899.0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29">
       <c r="A10">
         <v>457.9</v>
       </c>
@@ -5075,8 +6338,29 @@
       <c r="V10">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="11" spans="1:22">
+      <c r="W10">
+        <v>0.0</v>
+      </c>
+      <c r="X10">
+        <v>0.0</v>
+      </c>
+      <c r="Y10">
+        <v>0.0</v>
+      </c>
+      <c r="Z10">
+        <v>0.0</v>
+      </c>
+      <c r="AA10">
+        <v>0.0</v>
+      </c>
+      <c r="AB10">
+        <v>0.0</v>
+      </c>
+      <c r="AC10">
+        <v>11161.0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29">
       <c r="A11">
         <v>457.9</v>
       </c>
@@ -5143,8 +6427,29 @@
       <c r="V11">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="12" spans="1:22">
+      <c r="W11">
+        <v>0.0</v>
+      </c>
+      <c r="X11">
+        <v>0.0</v>
+      </c>
+      <c r="Y11">
+        <v>0.0</v>
+      </c>
+      <c r="Z11">
+        <v>0.0</v>
+      </c>
+      <c r="AA11">
+        <v>0.0</v>
+      </c>
+      <c r="AB11">
+        <v>0.0</v>
+      </c>
+      <c r="AC11">
+        <v>11463.0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29">
       <c r="A12">
         <v>457.9</v>
       </c>
@@ -5211,8 +6516,29 @@
       <c r="V12">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="13" spans="1:22">
+      <c r="W12">
+        <v>0.0</v>
+      </c>
+      <c r="X12">
+        <v>0.0</v>
+      </c>
+      <c r="Y12">
+        <v>0.0</v>
+      </c>
+      <c r="Z12">
+        <v>0.0</v>
+      </c>
+      <c r="AA12">
+        <v>0.0</v>
+      </c>
+      <c r="AB12">
+        <v>0.0</v>
+      </c>
+      <c r="AC12">
+        <v>11837.0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29">
       <c r="A13">
         <v>457.9</v>
       </c>
@@ -5279,8 +6605,29 @@
       <c r="V13">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="14" spans="1:22">
+      <c r="W13">
+        <v>0.0</v>
+      </c>
+      <c r="X13">
+        <v>0.0</v>
+      </c>
+      <c r="Y13">
+        <v>0.0</v>
+      </c>
+      <c r="Z13">
+        <v>0.0</v>
+      </c>
+      <c r="AA13">
+        <v>0.0</v>
+      </c>
+      <c r="AB13">
+        <v>0.0</v>
+      </c>
+      <c r="AC13">
+        <v>12258.0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29">
       <c r="A14">
         <v>457.9</v>
       </c>
@@ -5347,8 +6694,29 @@
       <c r="V14">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="15" spans="1:22">
+      <c r="W14">
+        <v>0.0</v>
+      </c>
+      <c r="X14">
+        <v>0.0</v>
+      </c>
+      <c r="Y14">
+        <v>0.0</v>
+      </c>
+      <c r="Z14">
+        <v>0.0</v>
+      </c>
+      <c r="AA14">
+        <v>0.0</v>
+      </c>
+      <c r="AB14">
+        <v>0.0</v>
+      </c>
+      <c r="AC14">
+        <v>12493.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29">
       <c r="A15">
         <v>457.9</v>
       </c>
@@ -5415,8 +6783,29 @@
       <c r="V15">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="16" spans="1:22">
+      <c r="W15">
+        <v>0.0</v>
+      </c>
+      <c r="X15">
+        <v>0.0</v>
+      </c>
+      <c r="Y15">
+        <v>0.0</v>
+      </c>
+      <c r="Z15">
+        <v>0.0</v>
+      </c>
+      <c r="AA15">
+        <v>0.0</v>
+      </c>
+      <c r="AB15">
+        <v>0.0</v>
+      </c>
+      <c r="AC15">
+        <v>12610.0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29">
       <c r="A16">
         <v>457.9</v>
       </c>
@@ -5483,8 +6872,29 @@
       <c r="V16">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="17" spans="1:22">
+      <c r="W16">
+        <v>0.0</v>
+      </c>
+      <c r="X16">
+        <v>0.0</v>
+      </c>
+      <c r="Y16">
+        <v>0.0</v>
+      </c>
+      <c r="Z16">
+        <v>0.0</v>
+      </c>
+      <c r="AA16">
+        <v>0.0</v>
+      </c>
+      <c r="AB16">
+        <v>0.0</v>
+      </c>
+      <c r="AC16">
+        <v>12587.0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29">
       <c r="A17">
         <v>457.9</v>
       </c>
@@ -5551,8 +6961,29 @@
       <c r="V17">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="18" spans="1:22">
+      <c r="W17">
+        <v>0.0</v>
+      </c>
+      <c r="X17">
+        <v>0.0</v>
+      </c>
+      <c r="Y17">
+        <v>0.0</v>
+      </c>
+      <c r="Z17">
+        <v>0.0</v>
+      </c>
+      <c r="AA17">
+        <v>0.0</v>
+      </c>
+      <c r="AB17">
+        <v>0.0</v>
+      </c>
+      <c r="AC17">
+        <v>12709.0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29">
       <c r="A18">
         <v>457.9</v>
       </c>
@@ -5619,8 +7050,29 @@
       <c r="V18">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="19" spans="1:22">
+      <c r="W18">
+        <v>0.0</v>
+      </c>
+      <c r="X18">
+        <v>0.0</v>
+      </c>
+      <c r="Y18">
+        <v>0.0</v>
+      </c>
+      <c r="Z18">
+        <v>0.0</v>
+      </c>
+      <c r="AA18">
+        <v>0.0</v>
+      </c>
+      <c r="AB18">
+        <v>0.0</v>
+      </c>
+      <c r="AC18">
+        <v>13077.0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29">
       <c r="A19">
         <v>457.9</v>
       </c>
@@ -5687,8 +7139,29 @@
       <c r="V19">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="20" spans="1:22">
+      <c r="W19">
+        <v>0.0</v>
+      </c>
+      <c r="X19">
+        <v>0.0</v>
+      </c>
+      <c r="Y19">
+        <v>0.0</v>
+      </c>
+      <c r="Z19">
+        <v>0.0</v>
+      </c>
+      <c r="AA19">
+        <v>0.0</v>
+      </c>
+      <c r="AB19">
+        <v>0.0</v>
+      </c>
+      <c r="AC19">
+        <v>14079.0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29">
       <c r="A20">
         <v>457.9</v>
       </c>
@@ -5755,8 +7228,29 @@
       <c r="V20">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="21" spans="1:22">
+      <c r="W20">
+        <v>0.0</v>
+      </c>
+      <c r="X20">
+        <v>0.0</v>
+      </c>
+      <c r="Y20">
+        <v>0.0</v>
+      </c>
+      <c r="Z20">
+        <v>0.0</v>
+      </c>
+      <c r="AA20">
+        <v>0.0</v>
+      </c>
+      <c r="AB20">
+        <v>0.0</v>
+      </c>
+      <c r="AC20">
+        <v>13950.0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29">
       <c r="A21">
         <v>457.9</v>
       </c>
@@ -5823,8 +7317,29 @@
       <c r="V21">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="22" spans="1:22">
+      <c r="W21">
+        <v>0.0</v>
+      </c>
+      <c r="X21">
+        <v>0.0</v>
+      </c>
+      <c r="Y21">
+        <v>0.0</v>
+      </c>
+      <c r="Z21">
+        <v>0.0</v>
+      </c>
+      <c r="AA21">
+        <v>0.0</v>
+      </c>
+      <c r="AB21">
+        <v>0.0</v>
+      </c>
+      <c r="AC21">
+        <v>13678.0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29">
       <c r="A22">
         <v>457.9</v>
       </c>
@@ -5891,8 +7406,29 @@
       <c r="V22">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="23" spans="1:22">
+      <c r="W22">
+        <v>0.0</v>
+      </c>
+      <c r="X22">
+        <v>0.0</v>
+      </c>
+      <c r="Y22">
+        <v>0.0</v>
+      </c>
+      <c r="Z22">
+        <v>0.0</v>
+      </c>
+      <c r="AA22">
+        <v>0.0</v>
+      </c>
+      <c r="AB22">
+        <v>0.0</v>
+      </c>
+      <c r="AC22">
+        <v>13311.0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29">
       <c r="A23">
         <v>457.9</v>
       </c>
@@ -5959,8 +7495,29 @@
       <c r="V23">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="24" spans="1:22">
+      <c r="W23">
+        <v>0.0</v>
+      </c>
+      <c r="X23">
+        <v>0.0</v>
+      </c>
+      <c r="Y23">
+        <v>0.0</v>
+      </c>
+      <c r="Z23">
+        <v>0.0</v>
+      </c>
+      <c r="AA23">
+        <v>0.0</v>
+      </c>
+      <c r="AB23">
+        <v>0.0</v>
+      </c>
+      <c r="AC23">
+        <v>12762.0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29">
       <c r="A24">
         <v>457.9</v>
       </c>
@@ -6027,8 +7584,29 @@
       <c r="V24">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="25" spans="1:22">
+      <c r="W24">
+        <v>0.0</v>
+      </c>
+      <c r="X24">
+        <v>0.0</v>
+      </c>
+      <c r="Y24">
+        <v>0.0</v>
+      </c>
+      <c r="Z24">
+        <v>0.0</v>
+      </c>
+      <c r="AA24">
+        <v>0.0</v>
+      </c>
+      <c r="AB24">
+        <v>0.0</v>
+      </c>
+      <c r="AC24">
+        <v>12222.0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29">
       <c r="A25">
         <v>457.9</v>
       </c>
@@ -6094,6 +7672,27 @@
       </c>
       <c r="V25">
         <v>0.0</v>
+      </c>
+      <c r="W25">
+        <v>0.0</v>
+      </c>
+      <c r="X25">
+        <v>0.0</v>
+      </c>
+      <c r="Y25">
+        <v>0.0</v>
+      </c>
+      <c r="Z25">
+        <v>0.0</v>
+      </c>
+      <c r="AA25">
+        <v>0.0</v>
+      </c>
+      <c r="AB25">
+        <v>0.0</v>
+      </c>
+      <c r="AC25">
+        <v>11522.0</v>
       </c>
     </row>
   </sheetData>
@@ -6103,13 +7702,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:V25"/>
+  <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6176,8 +7775,29 @@
       <c r="V1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:22">
+      <c r="W1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
       <c r="A2">
         <v>1767.0</v>
       </c>
@@ -6244,8 +7864,29 @@
       <c r="V2">
         <v>800.0</v>
       </c>
-    </row>
-    <row r="3" spans="1:22">
+      <c r="W2">
+        <v>0.0</v>
+      </c>
+      <c r="X2">
+        <v>0.0</v>
+      </c>
+      <c r="Y2">
+        <v>0.0</v>
+      </c>
+      <c r="Z2">
+        <v>0.0</v>
+      </c>
+      <c r="AA2">
+        <v>0.0</v>
+      </c>
+      <c r="AB2">
+        <v>0.0</v>
+      </c>
+      <c r="AC2">
+        <v>15011.51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29">
       <c r="A3">
         <v>1767.0</v>
       </c>
@@ -6312,8 +7953,29 @@
       <c r="V3">
         <v>800.0</v>
       </c>
-    </row>
-    <row r="4" spans="1:22">
+      <c r="W3">
+        <v>0.0</v>
+      </c>
+      <c r="X3">
+        <v>0.0</v>
+      </c>
+      <c r="Y3">
+        <v>0.0</v>
+      </c>
+      <c r="Z3">
+        <v>0.0</v>
+      </c>
+      <c r="AA3">
+        <v>0.0</v>
+      </c>
+      <c r="AB3">
+        <v>0.0</v>
+      </c>
+      <c r="AC3">
+        <v>14466.59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29">
       <c r="A4">
         <v>1767.0</v>
       </c>
@@ -6380,8 +8042,29 @@
       <c r="V4">
         <v>333.6999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:22">
+      <c r="W4">
+        <v>0.0</v>
+      </c>
+      <c r="X4">
+        <v>0.0</v>
+      </c>
+      <c r="Y4">
+        <v>0.0</v>
+      </c>
+      <c r="Z4">
+        <v>0.0</v>
+      </c>
+      <c r="AA4">
+        <v>0.0</v>
+      </c>
+      <c r="AB4">
+        <v>0.0</v>
+      </c>
+      <c r="AC4">
+        <v>13773.58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29">
       <c r="A5">
         <v>1767.0</v>
       </c>
@@ -6448,8 +8131,29 @@
       <c r="V5">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="6" spans="1:22">
+      <c r="W5">
+        <v>0.0</v>
+      </c>
+      <c r="X5">
+        <v>0.0</v>
+      </c>
+      <c r="Y5">
+        <v>0.0</v>
+      </c>
+      <c r="Z5">
+        <v>0.0</v>
+      </c>
+      <c r="AA5">
+        <v>0.0</v>
+      </c>
+      <c r="AB5">
+        <v>0.0</v>
+      </c>
+      <c r="AC5">
+        <v>13406.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29">
       <c r="A6">
         <v>1767.0</v>
       </c>
@@ -6516,8 +8220,29 @@
       <c r="V6">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="7" spans="1:22">
+      <c r="W6">
+        <v>0.0</v>
+      </c>
+      <c r="X6">
+        <v>0.0</v>
+      </c>
+      <c r="Y6">
+        <v>0.0</v>
+      </c>
+      <c r="Z6">
+        <v>0.0</v>
+      </c>
+      <c r="AA6">
+        <v>0.0</v>
+      </c>
+      <c r="AB6">
+        <v>505.43199999999956</v>
+      </c>
+      <c r="AC6">
+        <v>13216.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29">
       <c r="A7">
         <v>1767.0</v>
       </c>
@@ -6584,8 +8309,29 @@
       <c r="V7">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="8" spans="1:22">
+      <c r="W7">
+        <v>0.0</v>
+      </c>
+      <c r="X7">
+        <v>0.0</v>
+      </c>
+      <c r="Y7">
+        <v>0.0</v>
+      </c>
+      <c r="Z7">
+        <v>0.0</v>
+      </c>
+      <c r="AA7">
+        <v>0.0</v>
+      </c>
+      <c r="AB7">
+        <v>770.6159999999988</v>
+      </c>
+      <c r="AC7">
+        <v>13126.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29">
       <c r="A8">
         <v>1767.0</v>
       </c>
@@ -6652,8 +8398,29 @@
       <c r="V8">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="9" spans="1:22">
+      <c r="W8">
+        <v>0.0</v>
+      </c>
+      <c r="X8">
+        <v>0.0</v>
+      </c>
+      <c r="Y8">
+        <v>0.0</v>
+      </c>
+      <c r="Z8">
+        <v>0.0</v>
+      </c>
+      <c r="AA8">
+        <v>0.0</v>
+      </c>
+      <c r="AB8">
+        <v>800.0</v>
+      </c>
+      <c r="AC8">
+        <v>13215.61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29">
       <c r="A9">
         <v>1767.0</v>
       </c>
@@ -6720,8 +8487,29 @@
       <c r="V9">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="10" spans="1:22">
+      <c r="W9">
+        <v>0.0</v>
+      </c>
+      <c r="X9">
+        <v>0.0</v>
+      </c>
+      <c r="Y9">
+        <v>0.0</v>
+      </c>
+      <c r="Z9">
+        <v>0.0</v>
+      </c>
+      <c r="AA9">
+        <v>0.0</v>
+      </c>
+      <c r="AB9">
+        <v>800.0</v>
+      </c>
+      <c r="AC9">
+        <v>13087.74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29">
       <c r="A10">
         <v>1767.0</v>
       </c>
@@ -6788,8 +8576,29 @@
       <c r="V10">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="11" spans="1:22">
+      <c r="W10">
+        <v>0.0</v>
+      </c>
+      <c r="X10">
+        <v>0.0</v>
+      </c>
+      <c r="Y10">
+        <v>0.0</v>
+      </c>
+      <c r="Z10">
+        <v>0.0</v>
+      </c>
+      <c r="AA10">
+        <v>0.0</v>
+      </c>
+      <c r="AB10">
+        <v>463.1278029702985</v>
+      </c>
+      <c r="AC10">
+        <v>12992.96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29">
       <c r="A11">
         <v>1767.0</v>
       </c>
@@ -6856,8 +8665,29 @@
       <c r="V11">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="12" spans="1:22">
+      <c r="W11">
+        <v>0.0</v>
+      </c>
+      <c r="X11">
+        <v>0.0</v>
+      </c>
+      <c r="Y11">
+        <v>0.0</v>
+      </c>
+      <c r="Z11">
+        <v>0.0</v>
+      </c>
+      <c r="AA11">
+        <v>0.0</v>
+      </c>
+      <c r="AB11">
+        <v>800.0</v>
+      </c>
+      <c r="AC11">
+        <v>13425.55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29">
       <c r="A12">
         <v>1767.0</v>
       </c>
@@ -6924,8 +8754,29 @@
       <c r="V12">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="13" spans="1:22">
+      <c r="W12">
+        <v>0.0</v>
+      </c>
+      <c r="X12">
+        <v>0.0</v>
+      </c>
+      <c r="Y12">
+        <v>0.0</v>
+      </c>
+      <c r="Z12">
+        <v>0.0</v>
+      </c>
+      <c r="AA12">
+        <v>0.0</v>
+      </c>
+      <c r="AB12">
+        <v>0.0</v>
+      </c>
+      <c r="AC12">
+        <v>14082.94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29">
       <c r="A13">
         <v>1767.0</v>
       </c>
@@ -6992,8 +8843,29 @@
       <c r="V13">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="14" spans="1:22">
+      <c r="W13">
+        <v>0.0</v>
+      </c>
+      <c r="X13">
+        <v>0.0</v>
+      </c>
+      <c r="Y13">
+        <v>0.0</v>
+      </c>
+      <c r="Z13">
+        <v>0.0</v>
+      </c>
+      <c r="AA13">
+        <v>0.0</v>
+      </c>
+      <c r="AB13">
+        <v>91.55389999999966</v>
+      </c>
+      <c r="AC13">
+        <v>14688.34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29">
       <c r="A14">
         <v>1767.0</v>
       </c>
@@ -7060,8 +8932,29 @@
       <c r="V14">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="15" spans="1:22">
+      <c r="W14">
+        <v>0.0</v>
+      </c>
+      <c r="X14">
+        <v>0.0</v>
+      </c>
+      <c r="Y14">
+        <v>0.0</v>
+      </c>
+      <c r="Z14">
+        <v>0.0</v>
+      </c>
+      <c r="AA14">
+        <v>0.0</v>
+      </c>
+      <c r="AB14">
+        <v>0.0</v>
+      </c>
+      <c r="AC14">
+        <v>15234.81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29">
       <c r="A15">
         <v>1767.0</v>
       </c>
@@ -7128,8 +9021,29 @@
       <c r="V15">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="16" spans="1:22">
+      <c r="W15">
+        <v>0.0</v>
+      </c>
+      <c r="X15">
+        <v>0.0</v>
+      </c>
+      <c r="Y15">
+        <v>0.0</v>
+      </c>
+      <c r="Z15">
+        <v>0.0</v>
+      </c>
+      <c r="AA15">
+        <v>0.0</v>
+      </c>
+      <c r="AB15">
+        <v>0.0</v>
+      </c>
+      <c r="AC15">
+        <v>15708.93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29">
       <c r="A16">
         <v>1767.0</v>
       </c>
@@ -7196,8 +9110,29 @@
       <c r="V16">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="17" spans="1:22">
+      <c r="W16">
+        <v>0.0</v>
+      </c>
+      <c r="X16">
+        <v>0.0</v>
+      </c>
+      <c r="Y16">
+        <v>0.0</v>
+      </c>
+      <c r="Z16">
+        <v>0.0</v>
+      </c>
+      <c r="AA16">
+        <v>0.0</v>
+      </c>
+      <c r="AB16">
+        <v>0.0</v>
+      </c>
+      <c r="AC16">
+        <v>15801.49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29">
       <c r="A17">
         <v>1767.0</v>
       </c>
@@ -7264,8 +9199,29 @@
       <c r="V17">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="18" spans="1:22">
+      <c r="W17">
+        <v>0.0</v>
+      </c>
+      <c r="X17">
+        <v>0.0</v>
+      </c>
+      <c r="Y17">
+        <v>0.0</v>
+      </c>
+      <c r="Z17">
+        <v>0.0</v>
+      </c>
+      <c r="AA17">
+        <v>0.0</v>
+      </c>
+      <c r="AB17">
+        <v>0.0</v>
+      </c>
+      <c r="AC17">
+        <v>15845.06</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29">
       <c r="A18">
         <v>1767.0</v>
       </c>
@@ -7332,8 +9288,29 @@
       <c r="V18">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="19" spans="1:22">
+      <c r="W18">
+        <v>0.0</v>
+      </c>
+      <c r="X18">
+        <v>0.0</v>
+      </c>
+      <c r="Y18">
+        <v>0.0</v>
+      </c>
+      <c r="Z18">
+        <v>0.0</v>
+      </c>
+      <c r="AA18">
+        <v>0.0</v>
+      </c>
+      <c r="AB18">
+        <v>0.0</v>
+      </c>
+      <c r="AC18">
+        <v>16939.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29">
       <c r="A19">
         <v>1767.0</v>
       </c>
@@ -7400,8 +9377,29 @@
       <c r="V19">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="20" spans="1:22">
+      <c r="W19">
+        <v>0.0</v>
+      </c>
+      <c r="X19">
+        <v>0.0</v>
+      </c>
+      <c r="Y19">
+        <v>0.0</v>
+      </c>
+      <c r="Z19">
+        <v>0.0</v>
+      </c>
+      <c r="AA19">
+        <v>0.0</v>
+      </c>
+      <c r="AB19">
+        <v>0.0</v>
+      </c>
+      <c r="AC19">
+        <v>17255.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29">
       <c r="A20">
         <v>1767.0</v>
       </c>
@@ -7468,8 +9466,29 @@
       <c r="V20">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="21" spans="1:22">
+      <c r="W20">
+        <v>0.0</v>
+      </c>
+      <c r="X20">
+        <v>0.0</v>
+      </c>
+      <c r="Y20">
+        <v>0.0</v>
+      </c>
+      <c r="Z20">
+        <v>0.0</v>
+      </c>
+      <c r="AA20">
+        <v>0.0</v>
+      </c>
+      <c r="AB20">
+        <v>0.0</v>
+      </c>
+      <c r="AC20">
+        <v>17339.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29">
       <c r="A21">
         <v>1767.0</v>
       </c>
@@ -7536,8 +9555,29 @@
       <c r="V21">
         <v>800.0</v>
       </c>
-    </row>
-    <row r="22" spans="1:22">
+      <c r="W21">
+        <v>0.0</v>
+      </c>
+      <c r="X21">
+        <v>0.0</v>
+      </c>
+      <c r="Y21">
+        <v>0.0</v>
+      </c>
+      <c r="Z21">
+        <v>0.0</v>
+      </c>
+      <c r="AA21">
+        <v>0.0</v>
+      </c>
+      <c r="AB21">
+        <v>0.0</v>
+      </c>
+      <c r="AC21">
+        <v>17350.24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29">
       <c r="A22">
         <v>1767.0</v>
       </c>
@@ -7604,8 +9644,29 @@
       <c r="V22">
         <v>800.0</v>
       </c>
-    </row>
-    <row r="23" spans="1:22">
+      <c r="W22">
+        <v>0.0</v>
+      </c>
+      <c r="X22">
+        <v>0.0</v>
+      </c>
+      <c r="Y22">
+        <v>0.0</v>
+      </c>
+      <c r="Z22">
+        <v>0.0</v>
+      </c>
+      <c r="AA22">
+        <v>0.0</v>
+      </c>
+      <c r="AB22">
+        <v>0.0</v>
+      </c>
+      <c r="AC22">
+        <v>16974.09</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29">
       <c r="A23">
         <v>1767.0</v>
       </c>
@@ -7672,8 +9733,29 @@
       <c r="V23">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="24" spans="1:22">
+      <c r="W23">
+        <v>0.0</v>
+      </c>
+      <c r="X23">
+        <v>0.0</v>
+      </c>
+      <c r="Y23">
+        <v>0.0</v>
+      </c>
+      <c r="Z23">
+        <v>0.0</v>
+      </c>
+      <c r="AA23">
+        <v>0.0</v>
+      </c>
+      <c r="AB23">
+        <v>0.0</v>
+      </c>
+      <c r="AC23">
+        <v>16279.04</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29">
       <c r="A24">
         <v>1767.0</v>
       </c>
@@ -7740,8 +9822,29 @@
       <c r="V24">
         <v>697.029702970297</v>
       </c>
-    </row>
-    <row r="25" spans="1:22">
+      <c r="W24">
+        <v>0.0</v>
+      </c>
+      <c r="X24">
+        <v>0.0</v>
+      </c>
+      <c r="Y24">
+        <v>0.0</v>
+      </c>
+      <c r="Z24">
+        <v>0.0</v>
+      </c>
+      <c r="AA24">
+        <v>0.0</v>
+      </c>
+      <c r="AB24">
+        <v>0.0</v>
+      </c>
+      <c r="AC24">
+        <v>15653.89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29">
       <c r="A25">
         <v>1767.0</v>
       </c>
@@ -7807,6 +9910,27 @@
       </c>
       <c r="V25">
         <v>0.0</v>
+      </c>
+      <c r="W25">
+        <v>0.0</v>
+      </c>
+      <c r="X25">
+        <v>0.0</v>
+      </c>
+      <c r="Y25">
+        <v>0.0</v>
+      </c>
+      <c r="Z25">
+        <v>0.0</v>
+      </c>
+      <c r="AA25">
+        <v>0.0</v>
+      </c>
+      <c r="AB25">
+        <v>0.0</v>
+      </c>
+      <c r="AC25">
+        <v>14593.1</v>
       </c>
     </row>
   </sheetData>
@@ -7816,13 +9940,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:V25"/>
+  <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7889,8 +10013,29 @@
       <c r="V1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:22">
+      <c r="W1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
       <c r="A2">
         <v>2943.3500000000004</v>
       </c>
@@ -7957,8 +10102,29 @@
       <c r="V2">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="3" spans="1:22">
+      <c r="W2">
+        <v>450.0</v>
+      </c>
+      <c r="X2">
+        <v>0.0</v>
+      </c>
+      <c r="Y2">
+        <v>0.0</v>
+      </c>
+      <c r="Z2">
+        <v>0.0</v>
+      </c>
+      <c r="AA2">
+        <v>1200.0</v>
+      </c>
+      <c r="AB2">
+        <v>0.0</v>
+      </c>
+      <c r="AC2">
+        <v>14597.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29">
       <c r="A3">
         <v>2611.938888888889</v>
       </c>
@@ -8025,8 +10191,29 @@
       <c r="V3">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="4" spans="1:22">
+      <c r="W3">
+        <v>450.0</v>
+      </c>
+      <c r="X3">
+        <v>0.0</v>
+      </c>
+      <c r="Y3">
+        <v>0.0</v>
+      </c>
+      <c r="Z3">
+        <v>0.0</v>
+      </c>
+      <c r="AA3">
+        <v>969.5888888888876</v>
+      </c>
+      <c r="AB3">
+        <v>0.0</v>
+      </c>
+      <c r="AC3">
+        <v>14375.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29">
       <c r="A4">
         <v>1193.3500000000004</v>
       </c>
@@ -8093,8 +10280,29 @@
       <c r="V4">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="5" spans="1:22">
+      <c r="W4">
+        <v>0.0</v>
+      </c>
+      <c r="X4">
+        <v>0.0</v>
+      </c>
+      <c r="Y4">
+        <v>0.0</v>
+      </c>
+      <c r="Z4">
+        <v>0.0</v>
+      </c>
+      <c r="AA4">
+        <v>0.0</v>
+      </c>
+      <c r="AB4">
+        <v>0.0</v>
+      </c>
+      <c r="AC4">
+        <v>14153.0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29">
       <c r="A5">
         <v>1013.3500000000004</v>
       </c>
@@ -8161,8 +10369,29 @@
       <c r="V5">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="6" spans="1:22">
+      <c r="W5">
+        <v>0.0</v>
+      </c>
+      <c r="X5">
+        <v>0.0</v>
+      </c>
+      <c r="Y5">
+        <v>0.0</v>
+      </c>
+      <c r="Z5">
+        <v>0.0</v>
+      </c>
+      <c r="AA5">
+        <v>0.0</v>
+      </c>
+      <c r="AB5">
+        <v>0.0</v>
+      </c>
+      <c r="AC5">
+        <v>13896.0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29">
       <c r="A6">
         <v>1111.3499999999995</v>
       </c>
@@ -8229,8 +10458,29 @@
       <c r="V6">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="7" spans="1:22">
+      <c r="W6">
+        <v>0.0</v>
+      </c>
+      <c r="X6">
+        <v>0.0</v>
+      </c>
+      <c r="Y6">
+        <v>0.0</v>
+      </c>
+      <c r="Z6">
+        <v>0.0</v>
+      </c>
+      <c r="AA6">
+        <v>0.0</v>
+      </c>
+      <c r="AB6">
+        <v>0.0</v>
+      </c>
+      <c r="AC6">
+        <v>13955.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29">
       <c r="A7">
         <v>1323.3500000000004</v>
       </c>
@@ -8297,8 +10547,29 @@
       <c r="V7">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="8" spans="1:22">
+      <c r="W7">
+        <v>0.0</v>
+      </c>
+      <c r="X7">
+        <v>0.0</v>
+      </c>
+      <c r="Y7">
+        <v>0.0</v>
+      </c>
+      <c r="Z7">
+        <v>0.0</v>
+      </c>
+      <c r="AA7">
+        <v>0.0</v>
+      </c>
+      <c r="AB7">
+        <v>0.0</v>
+      </c>
+      <c r="AC7">
+        <v>14166.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29">
       <c r="A8">
         <v>1567.3500000000004</v>
       </c>
@@ -8365,8 +10636,29 @@
       <c r="V8">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="9" spans="1:22">
+      <c r="W8">
+        <v>0.0</v>
+      </c>
+      <c r="X8">
+        <v>0.0</v>
+      </c>
+      <c r="Y8">
+        <v>0.0</v>
+      </c>
+      <c r="Z8">
+        <v>0.0</v>
+      </c>
+      <c r="AA8">
+        <v>0.0</v>
+      </c>
+      <c r="AB8">
+        <v>0.0</v>
+      </c>
+      <c r="AC8">
+        <v>14352.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29">
       <c r="A9">
         <v>1958.3499999999995</v>
       </c>
@@ -8433,8 +10725,29 @@
       <c r="V9">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="10" spans="1:22">
+      <c r="W9">
+        <v>0.0</v>
+      </c>
+      <c r="X9">
+        <v>0.0</v>
+      </c>
+      <c r="Y9">
+        <v>0.0</v>
+      </c>
+      <c r="Z9">
+        <v>0.0</v>
+      </c>
+      <c r="AA9">
+        <v>0.0</v>
+      </c>
+      <c r="AB9">
+        <v>0.0</v>
+      </c>
+      <c r="AC9">
+        <v>14807.0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29">
       <c r="A10">
         <v>2085.3500000000004</v>
       </c>
@@ -8501,8 +10814,29 @@
       <c r="V10">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="11" spans="1:22">
+      <c r="W10">
+        <v>0.0</v>
+      </c>
+      <c r="X10">
+        <v>0.0</v>
+      </c>
+      <c r="Y10">
+        <v>0.0</v>
+      </c>
+      <c r="Z10">
+        <v>0.0</v>
+      </c>
+      <c r="AA10">
+        <v>0.0</v>
+      </c>
+      <c r="AB10">
+        <v>0.0</v>
+      </c>
+      <c r="AC10">
+        <v>15064.0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29">
       <c r="A11">
         <v>2469.3500000000004</v>
       </c>
@@ -8569,8 +10903,29 @@
       <c r="V11">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="12" spans="1:22">
+      <c r="W11">
+        <v>0.0</v>
+      </c>
+      <c r="X11">
+        <v>0.0</v>
+      </c>
+      <c r="Y11">
+        <v>0.0</v>
+      </c>
+      <c r="Z11">
+        <v>0.0</v>
+      </c>
+      <c r="AA11">
+        <v>0.0</v>
+      </c>
+      <c r="AB11">
+        <v>0.0</v>
+      </c>
+      <c r="AC11">
+        <v>15492.0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29">
       <c r="A12">
         <v>3829.3500000000004</v>
       </c>
@@ -8637,8 +10992,29 @@
       <c r="V12">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="13" spans="1:22">
+      <c r="W12">
+        <v>0.0</v>
+      </c>
+      <c r="X12">
+        <v>0.0</v>
+      </c>
+      <c r="Y12">
+        <v>0.0</v>
+      </c>
+      <c r="Z12">
+        <v>0.0</v>
+      </c>
+      <c r="AA12">
+        <v>1200.0</v>
+      </c>
+      <c r="AB12">
+        <v>0.0</v>
+      </c>
+      <c r="AC12">
+        <v>15810.0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29">
       <c r="A13">
         <v>2763.8499999999967</v>
       </c>
@@ -8705,8 +11081,29 @@
       <c r="V13">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="14" spans="1:22">
+      <c r="W13">
+        <v>0.0</v>
+      </c>
+      <c r="X13">
+        <v>0.0</v>
+      </c>
+      <c r="Y13">
+        <v>0.0</v>
+      </c>
+      <c r="Z13">
+        <v>0.0</v>
+      </c>
+      <c r="AA13">
+        <v>126.49999999999613</v>
+      </c>
+      <c r="AB13">
+        <v>0.0</v>
+      </c>
+      <c r="AC13">
+        <v>16045.0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29">
       <c r="A14">
         <v>3874.3500000000004</v>
       </c>
@@ -8773,8 +11170,29 @@
       <c r="V14">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="15" spans="1:22">
+      <c r="W14">
+        <v>0.0</v>
+      </c>
+      <c r="X14">
+        <v>0.0</v>
+      </c>
+      <c r="Y14">
+        <v>0.0</v>
+      </c>
+      <c r="Z14">
+        <v>0.0</v>
+      </c>
+      <c r="AA14">
+        <v>1200.0</v>
+      </c>
+      <c r="AB14">
+        <v>0.0</v>
+      </c>
+      <c r="AC14">
+        <v>16254.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29">
       <c r="A15">
         <v>3825.3500000000004</v>
       </c>
@@ -8841,8 +11259,29 @@
       <c r="V15">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="16" spans="1:22">
+      <c r="W15">
+        <v>0.0</v>
+      </c>
+      <c r="X15">
+        <v>0.0</v>
+      </c>
+      <c r="Y15">
+        <v>0.0</v>
+      </c>
+      <c r="Z15">
+        <v>0.0</v>
+      </c>
+      <c r="AA15">
+        <v>1200.0</v>
+      </c>
+      <c r="AB15">
+        <v>0.0</v>
+      </c>
+      <c r="AC15">
+        <v>16321.0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29">
       <c r="A16">
         <v>4176.349999999999</v>
       </c>
@@ -8909,8 +11348,29 @@
       <c r="V16">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="17" spans="1:22">
+      <c r="W16">
+        <v>0.0</v>
+      </c>
+      <c r="X16">
+        <v>0.0</v>
+      </c>
+      <c r="Y16">
+        <v>0.0</v>
+      </c>
+      <c r="Z16">
+        <v>0.0</v>
+      </c>
+      <c r="AA16">
+        <v>1200.0</v>
+      </c>
+      <c r="AB16">
+        <v>0.0</v>
+      </c>
+      <c r="AC16">
+        <v>16874.0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29">
       <c r="A17">
         <v>4632.35</v>
       </c>
@@ -8977,8 +11437,29 @@
       <c r="V17">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="18" spans="1:22">
+      <c r="W17">
+        <v>0.0</v>
+      </c>
+      <c r="X17">
+        <v>0.0</v>
+      </c>
+      <c r="Y17">
+        <v>0.0</v>
+      </c>
+      <c r="Z17">
+        <v>0.0</v>
+      </c>
+      <c r="AA17">
+        <v>1200.0</v>
+      </c>
+      <c r="AB17">
+        <v>0.0</v>
+      </c>
+      <c r="AC17">
+        <v>17436.0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29">
       <c r="A18">
         <v>5316.35</v>
       </c>
@@ -9045,8 +11526,29 @@
       <c r="V18">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="19" spans="1:22">
+      <c r="W18">
+        <v>0.0</v>
+      </c>
+      <c r="X18">
+        <v>0.0</v>
+      </c>
+      <c r="Y18">
+        <v>0.0</v>
+      </c>
+      <c r="Z18">
+        <v>0.0</v>
+      </c>
+      <c r="AA18">
+        <v>1200.0</v>
+      </c>
+      <c r="AB18">
+        <v>0.0</v>
+      </c>
+      <c r="AC18">
+        <v>18173.0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29">
       <c r="A19">
         <v>5921.35</v>
       </c>
@@ -9113,8 +11615,29 @@
       <c r="V19">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="20" spans="1:22">
+      <c r="W19">
+        <v>450.0</v>
+      </c>
+      <c r="X19">
+        <v>0.0</v>
+      </c>
+      <c r="Y19">
+        <v>0.0</v>
+      </c>
+      <c r="Z19">
+        <v>0.0</v>
+      </c>
+      <c r="AA19">
+        <v>1200.0</v>
+      </c>
+      <c r="AB19">
+        <v>0.0</v>
+      </c>
+      <c r="AC19">
+        <v>18388.0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29">
       <c r="A20">
         <v>5705.35</v>
       </c>
@@ -9181,8 +11704,29 @@
       <c r="V20">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="21" spans="1:22">
+      <c r="W20">
+        <v>450.0</v>
+      </c>
+      <c r="X20">
+        <v>0.0</v>
+      </c>
+      <c r="Y20">
+        <v>0.0</v>
+      </c>
+      <c r="Z20">
+        <v>0.0</v>
+      </c>
+      <c r="AA20">
+        <v>1200.0</v>
+      </c>
+      <c r="AB20">
+        <v>0.0</v>
+      </c>
+      <c r="AC20">
+        <v>18200.0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29">
       <c r="A21">
         <v>5194.35</v>
       </c>
@@ -9249,8 +11793,29 @@
       <c r="V21">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="22" spans="1:22">
+      <c r="W21">
+        <v>450.0</v>
+      </c>
+      <c r="X21">
+        <v>0.0</v>
+      </c>
+      <c r="Y21">
+        <v>0.0</v>
+      </c>
+      <c r="Z21">
+        <v>0.0</v>
+      </c>
+      <c r="AA21">
+        <v>1200.0</v>
+      </c>
+      <c r="AB21">
+        <v>0.0</v>
+      </c>
+      <c r="AC21">
+        <v>17725.0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29">
       <c r="A22">
         <v>4425.35</v>
       </c>
@@ -9317,8 +11882,29 @@
       <c r="V22">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="23" spans="1:22">
+      <c r="W22">
+        <v>0.0</v>
+      </c>
+      <c r="X22">
+        <v>0.0</v>
+      </c>
+      <c r="Y22">
+        <v>0.0</v>
+      </c>
+      <c r="Z22">
+        <v>0.0</v>
+      </c>
+      <c r="AA22">
+        <v>1200.0</v>
+      </c>
+      <c r="AB22">
+        <v>0.0</v>
+      </c>
+      <c r="AC22">
+        <v>17424.0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29">
       <c r="A23">
         <v>4038.3499999999995</v>
       </c>
@@ -9385,8 +11971,29 @@
       <c r="V23">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="24" spans="1:22">
+      <c r="W23">
+        <v>0.0</v>
+      </c>
+      <c r="X23">
+        <v>0.0</v>
+      </c>
+      <c r="Y23">
+        <v>0.0</v>
+      </c>
+      <c r="Z23">
+        <v>0.0</v>
+      </c>
+      <c r="AA23">
+        <v>1200.0</v>
+      </c>
+      <c r="AB23">
+        <v>0.0</v>
+      </c>
+      <c r="AC23">
+        <v>17030.0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29">
       <c r="A24">
         <v>2569.3500000000004</v>
       </c>
@@ -9453,8 +12060,29 @@
       <c r="V24">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="25" spans="1:22">
+      <c r="W24">
+        <v>0.0</v>
+      </c>
+      <c r="X24">
+        <v>0.0</v>
+      </c>
+      <c r="Y24">
+        <v>0.0</v>
+      </c>
+      <c r="Z24">
+        <v>0.0</v>
+      </c>
+      <c r="AA24">
+        <v>0.0</v>
+      </c>
+      <c r="AB24">
+        <v>0.0</v>
+      </c>
+      <c r="AC24">
+        <v>16745.0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29">
       <c r="A25">
         <v>2187.3500000000004</v>
       </c>
@@ -9520,6 +12148,27 @@
       </c>
       <c r="V25">
         <v>0.0</v>
+      </c>
+      <c r="W25">
+        <v>0.0</v>
+      </c>
+      <c r="X25">
+        <v>0.0</v>
+      </c>
+      <c r="Y25">
+        <v>0.0</v>
+      </c>
+      <c r="Z25">
+        <v>0.0</v>
+      </c>
+      <c r="AA25">
+        <v>0.0</v>
+      </c>
+      <c r="AB25">
+        <v>0.0</v>
+      </c>
+      <c r="AC25">
+        <v>16335.0</v>
       </c>
     </row>
   </sheetData>
@@ -9529,13 +12178,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:V25"/>
+  <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9602,8 +12251,29 @@
       <c r="V1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:22">
+      <c r="W1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
       <c r="A2">
         <v>0.0</v>
       </c>
@@ -9670,8 +12340,29 @@
       <c r="V2">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="3" spans="1:22">
+      <c r="W2">
+        <v>1232.979999999999</v>
+      </c>
+      <c r="X2">
+        <v>0.0</v>
+      </c>
+      <c r="Y2">
+        <v>0.0</v>
+      </c>
+      <c r="Z2">
+        <v>0.0</v>
+      </c>
+      <c r="AA2">
+        <v>0.0</v>
+      </c>
+      <c r="AB2">
+        <v>0.0</v>
+      </c>
+      <c r="AC2">
+        <v>16008.04</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29">
       <c r="A3">
         <v>0.0</v>
       </c>
@@ -9738,8 +12429,29 @@
       <c r="V3">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="4" spans="1:22">
+      <c r="W3">
+        <v>1400.0</v>
+      </c>
+      <c r="X3">
+        <v>0.0</v>
+      </c>
+      <c r="Y3">
+        <v>0.0</v>
+      </c>
+      <c r="Z3">
+        <v>0.0</v>
+      </c>
+      <c r="AA3">
+        <v>0.0</v>
+      </c>
+      <c r="AB3">
+        <v>0.0</v>
+      </c>
+      <c r="AC3">
+        <v>15623.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29">
       <c r="A4">
         <v>0.0</v>
       </c>
@@ -9806,8 +12518,29 @@
       <c r="V4">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="5" spans="1:22">
+      <c r="W4">
+        <v>0.0</v>
+      </c>
+      <c r="X4">
+        <v>0.0</v>
+      </c>
+      <c r="Y4">
+        <v>0.0</v>
+      </c>
+      <c r="Z4">
+        <v>0.0</v>
+      </c>
+      <c r="AA4">
+        <v>0.0</v>
+      </c>
+      <c r="AB4">
+        <v>367.8719999999994</v>
+      </c>
+      <c r="AC4">
+        <v>15705.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29">
       <c r="A5">
         <v>0.0</v>
       </c>
@@ -9874,8 +12607,29 @@
       <c r="V5">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="6" spans="1:22">
+      <c r="W5">
+        <v>0.0</v>
+      </c>
+      <c r="X5">
+        <v>0.0</v>
+      </c>
+      <c r="Y5">
+        <v>0.0</v>
+      </c>
+      <c r="Z5">
+        <v>0.0</v>
+      </c>
+      <c r="AA5">
+        <v>0.0</v>
+      </c>
+      <c r="AB5">
+        <v>401.08799999999883</v>
+      </c>
+      <c r="AC5">
+        <v>15643.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29">
       <c r="A6">
         <v>0.0</v>
       </c>
@@ -9942,8 +12696,29 @@
       <c r="V6">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="7" spans="1:22">
+      <c r="W6">
+        <v>0.0</v>
+      </c>
+      <c r="X6">
+        <v>0.0</v>
+      </c>
+      <c r="Y6">
+        <v>0.0</v>
+      </c>
+      <c r="Z6">
+        <v>0.0</v>
+      </c>
+      <c r="AA6">
+        <v>0.0</v>
+      </c>
+      <c r="AB6">
+        <v>389.5119999999995</v>
+      </c>
+      <c r="AC6">
+        <v>15611.51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29">
       <c r="A7">
         <v>0.0</v>
       </c>
@@ -10010,8 +12785,29 @@
       <c r="V7">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="8" spans="1:22">
+      <c r="W7">
+        <v>0.0</v>
+      </c>
+      <c r="X7">
+        <v>0.0</v>
+      </c>
+      <c r="Y7">
+        <v>0.0</v>
+      </c>
+      <c r="Z7">
+        <v>0.0</v>
+      </c>
+      <c r="AA7">
+        <v>0.0</v>
+      </c>
+      <c r="AB7">
+        <v>273.80799999999954</v>
+      </c>
+      <c r="AC7">
+        <v>15727.76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29">
       <c r="A8">
         <v>0.0</v>
       </c>
@@ -10078,8 +12874,29 @@
       <c r="V8">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="9" spans="1:22">
+      <c r="W8">
+        <v>0.0</v>
+      </c>
+      <c r="X8">
+        <v>0.0</v>
+      </c>
+      <c r="Y8">
+        <v>0.0</v>
+      </c>
+      <c r="Z8">
+        <v>0.0</v>
+      </c>
+      <c r="AA8">
+        <v>0.0</v>
+      </c>
+      <c r="AB8">
+        <v>30.159999999999513</v>
+      </c>
+      <c r="AC8">
+        <v>16040.26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29">
       <c r="A9">
         <v>0.0</v>
       </c>
@@ -10146,8 +12963,29 @@
       <c r="V9">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="10" spans="1:22">
+      <c r="W9">
+        <v>0.0</v>
+      </c>
+      <c r="X9">
+        <v>0.0</v>
+      </c>
+      <c r="Y9">
+        <v>0.0</v>
+      </c>
+      <c r="Z9">
+        <v>0.0</v>
+      </c>
+      <c r="AA9">
+        <v>0.0</v>
+      </c>
+      <c r="AB9">
+        <v>0.0</v>
+      </c>
+      <c r="AC9">
+        <v>16324.51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29">
       <c r="A10">
         <v>0.0</v>
       </c>
@@ -10214,8 +13052,29 @@
       <c r="V10">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="11" spans="1:22">
+      <c r="W10">
+        <v>0.0</v>
+      </c>
+      <c r="X10">
+        <v>0.0</v>
+      </c>
+      <c r="Y10">
+        <v>0.0</v>
+      </c>
+      <c r="Z10">
+        <v>0.0</v>
+      </c>
+      <c r="AA10">
+        <v>0.0</v>
+      </c>
+      <c r="AB10">
+        <v>0.0</v>
+      </c>
+      <c r="AC10">
+        <v>16654.26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29">
       <c r="A11">
         <v>0.0</v>
       </c>
@@ -10282,8 +13141,29 @@
       <c r="V11">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="12" spans="1:22">
+      <c r="W11">
+        <v>0.0</v>
+      </c>
+      <c r="X11">
+        <v>0.0</v>
+      </c>
+      <c r="Y11">
+        <v>0.0</v>
+      </c>
+      <c r="Z11">
+        <v>0.0</v>
+      </c>
+      <c r="AA11">
+        <v>0.0</v>
+      </c>
+      <c r="AB11">
+        <v>0.0</v>
+      </c>
+      <c r="AC11">
+        <v>16935.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29">
       <c r="A12">
         <v>0.0</v>
       </c>
@@ -10350,8 +13230,29 @@
       <c r="V12">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="13" spans="1:22">
+      <c r="W12">
+        <v>0.0</v>
+      </c>
+      <c r="X12">
+        <v>0.0</v>
+      </c>
+      <c r="Y12">
+        <v>0.0</v>
+      </c>
+      <c r="Z12">
+        <v>0.0</v>
+      </c>
+      <c r="AA12">
+        <v>0.0</v>
+      </c>
+      <c r="AB12">
+        <v>0.0</v>
+      </c>
+      <c r="AC12">
+        <v>17369.26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29">
       <c r="A13">
         <v>0.0</v>
       </c>
@@ -10418,8 +13319,29 @@
       <c r="V13">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="14" spans="1:22">
+      <c r="W13">
+        <v>0.0</v>
+      </c>
+      <c r="X13">
+        <v>0.0</v>
+      </c>
+      <c r="Y13">
+        <v>0.0</v>
+      </c>
+      <c r="Z13">
+        <v>0.0</v>
+      </c>
+      <c r="AA13">
+        <v>0.0</v>
+      </c>
+      <c r="AB13">
+        <v>0.0</v>
+      </c>
+      <c r="AC13">
+        <v>17612.01</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29">
       <c r="A14">
         <v>0.0</v>
       </c>
@@ -10486,8 +13408,29 @@
       <c r="V14">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="15" spans="1:22">
+      <c r="W14">
+        <v>0.0</v>
+      </c>
+      <c r="X14">
+        <v>0.0</v>
+      </c>
+      <c r="Y14">
+        <v>0.0</v>
+      </c>
+      <c r="Z14">
+        <v>0.0</v>
+      </c>
+      <c r="AA14">
+        <v>0.0</v>
+      </c>
+      <c r="AB14">
+        <v>0.0</v>
+      </c>
+      <c r="AC14">
+        <v>17737.26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29">
       <c r="A15">
         <v>0.0</v>
       </c>
@@ -10554,8 +13497,29 @@
       <c r="V15">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="16" spans="1:22">
+      <c r="W15">
+        <v>0.0</v>
+      </c>
+      <c r="X15">
+        <v>0.0</v>
+      </c>
+      <c r="Y15">
+        <v>0.0</v>
+      </c>
+      <c r="Z15">
+        <v>0.0</v>
+      </c>
+      <c r="AA15">
+        <v>0.0</v>
+      </c>
+      <c r="AB15">
+        <v>0.0</v>
+      </c>
+      <c r="AC15">
+        <v>17688.76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29">
       <c r="A16">
         <v>0.0</v>
       </c>
@@ -10622,8 +13586,29 @@
       <c r="V16">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="17" spans="1:22">
+      <c r="W16">
+        <v>0.0</v>
+      </c>
+      <c r="X16">
+        <v>0.0</v>
+      </c>
+      <c r="Y16">
+        <v>0.0</v>
+      </c>
+      <c r="Z16">
+        <v>0.0</v>
+      </c>
+      <c r="AA16">
+        <v>0.0</v>
+      </c>
+      <c r="AB16">
+        <v>248.20937672000218</v>
+      </c>
+      <c r="AC16">
+        <v>18081.01</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29">
       <c r="A17">
         <v>0.0</v>
       </c>
@@ -10690,8 +13675,29 @@
       <c r="V17">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="18" spans="1:22">
+      <c r="W17">
+        <v>0.0</v>
+      </c>
+      <c r="X17">
+        <v>0.0</v>
+      </c>
+      <c r="Y17">
+        <v>0.0</v>
+      </c>
+      <c r="Z17">
+        <v>0.0</v>
+      </c>
+      <c r="AA17">
+        <v>0.0</v>
+      </c>
+      <c r="AB17">
+        <v>81.35199999999895</v>
+      </c>
+      <c r="AC17">
+        <v>18479.75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29">
       <c r="A18">
         <v>0.0</v>
       </c>
@@ -10758,8 +13764,29 @@
       <c r="V18">
         <v>61.01999999999839</v>
       </c>
-    </row>
-    <row r="19" spans="1:22">
+      <c r="W18">
+        <v>0.0</v>
+      </c>
+      <c r="X18">
+        <v>0.0</v>
+      </c>
+      <c r="Y18">
+        <v>0.0</v>
+      </c>
+      <c r="Z18">
+        <v>0.0</v>
+      </c>
+      <c r="AA18">
+        <v>0.0</v>
+      </c>
+      <c r="AB18">
+        <v>0.0</v>
+      </c>
+      <c r="AC18">
+        <v>18652.51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29">
       <c r="A19">
         <v>0.0</v>
       </c>
@@ -10826,8 +13853,29 @@
       <c r="V19">
         <v>46.23999999999842</v>
       </c>
-    </row>
-    <row r="20" spans="1:22">
+      <c r="W19">
+        <v>0.0</v>
+      </c>
+      <c r="X19">
+        <v>0.0</v>
+      </c>
+      <c r="Y19">
+        <v>0.0</v>
+      </c>
+      <c r="Z19">
+        <v>0.0</v>
+      </c>
+      <c r="AA19">
+        <v>0.0</v>
+      </c>
+      <c r="AB19">
+        <v>0.0</v>
+      </c>
+      <c r="AC19">
+        <v>18629.76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29">
       <c r="A20">
         <v>0.0</v>
       </c>
@@ -10894,8 +13942,29 @@
       <c r="V20">
         <v>1163.75</v>
       </c>
-    </row>
-    <row r="21" spans="1:22">
+      <c r="W20">
+        <v>0.0</v>
+      </c>
+      <c r="X20">
+        <v>0.0</v>
+      </c>
+      <c r="Y20">
+        <v>0.0</v>
+      </c>
+      <c r="Z20">
+        <v>0.0</v>
+      </c>
+      <c r="AA20">
+        <v>0.0</v>
+      </c>
+      <c r="AB20">
+        <v>0.0</v>
+      </c>
+      <c r="AC20">
+        <v>18492.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29">
       <c r="A21">
         <v>0.0</v>
       </c>
@@ -10962,8 +14031,29 @@
       <c r="V21">
         <v>880.7399999999984</v>
       </c>
-    </row>
-    <row r="22" spans="1:22">
+      <c r="W21">
+        <v>0.0</v>
+      </c>
+      <c r="X21">
+        <v>0.0</v>
+      </c>
+      <c r="Y21">
+        <v>0.0</v>
+      </c>
+      <c r="Z21">
+        <v>0.0</v>
+      </c>
+      <c r="AA21">
+        <v>0.0</v>
+      </c>
+      <c r="AB21">
+        <v>0.0</v>
+      </c>
+      <c r="AC21">
+        <v>18192.26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29">
       <c r="A22">
         <v>0.0</v>
       </c>
@@ -11030,8 +14120,29 @@
       <c r="V22">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="23" spans="1:22">
+      <c r="W22">
+        <v>0.0</v>
+      </c>
+      <c r="X22">
+        <v>0.0</v>
+      </c>
+      <c r="Y22">
+        <v>0.0</v>
+      </c>
+      <c r="Z22">
+        <v>0.0</v>
+      </c>
+      <c r="AA22">
+        <v>0.0</v>
+      </c>
+      <c r="AB22">
+        <v>359.74862327999676</v>
+      </c>
+      <c r="AC22">
+        <v>18035.01</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29">
       <c r="A23">
         <v>0.0</v>
       </c>
@@ -11098,8 +14209,29 @@
       <c r="V23">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="24" spans="1:22">
+      <c r="W23">
+        <v>0.0</v>
+      </c>
+      <c r="X23">
+        <v>0.0</v>
+      </c>
+      <c r="Y23">
+        <v>0.0</v>
+      </c>
+      <c r="Z23">
+        <v>0.0</v>
+      </c>
+      <c r="AA23">
+        <v>0.0</v>
+      </c>
+      <c r="AB23">
+        <v>0.0</v>
+      </c>
+      <c r="AC23">
+        <v>17631.26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29">
       <c r="A24">
         <v>0.0</v>
       </c>
@@ -11166,8 +14298,29 @@
       <c r="V24">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="25" spans="1:22">
+      <c r="W24">
+        <v>0.0</v>
+      </c>
+      <c r="X24">
+        <v>0.0</v>
+      </c>
+      <c r="Y24">
+        <v>0.0</v>
+      </c>
+      <c r="Z24">
+        <v>0.0</v>
+      </c>
+      <c r="AA24">
+        <v>0.0</v>
+      </c>
+      <c r="AB24">
+        <v>0.0</v>
+      </c>
+      <c r="AC24">
+        <v>17235.76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29">
       <c r="A25">
         <v>0.0</v>
       </c>
@@ -11233,6 +14386,27 @@
       </c>
       <c r="V25">
         <v>0.0</v>
+      </c>
+      <c r="W25">
+        <v>0.0</v>
+      </c>
+      <c r="X25">
+        <v>0.0</v>
+      </c>
+      <c r="Y25">
+        <v>0.0</v>
+      </c>
+      <c r="Z25">
+        <v>0.0</v>
+      </c>
+      <c r="AA25">
+        <v>0.0</v>
+      </c>
+      <c r="AB25">
+        <v>0.0</v>
+      </c>
+      <c r="AC25">
+        <v>17249.64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>